<commit_message>
Integrated reading data from xls sheet
Integrated reading data from xls sheet to the base class(DeviceName,
OSVersion, OSType)
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20400" windowHeight="9960" activeTab="2"/>
+    <workbookView windowWidth="20370" windowHeight="7980" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
   <si>
     <t>TCID</t>
   </si>
@@ -112,19 +112,52 @@
     <t>iii</t>
   </si>
   <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Device ID</t>
+    <t>DeviceName</t>
+  </si>
+  <si>
+    <t>DeviceID</t>
   </si>
   <si>
     <t>OS Name</t>
   </si>
   <si>
-    <t>OS Version</t>
+    <t>OSVersion</t>
   </si>
   <si>
     <t>Browser</t>
+  </si>
+  <si>
+    <t>OSType</t>
+  </si>
+  <si>
+    <t>Samsung Tab White</t>
+  </si>
+  <si>
+    <t>e9b94aea1ca24f6a</t>
+  </si>
+  <si>
+    <t>Marshmallow</t>
+  </si>
+  <si>
+    <t>6.0.1</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>Samsung Tab Black</t>
+  </si>
+  <si>
+    <t>64cd1224</t>
+  </si>
+  <si>
+    <t>Lollipop</t>
+  </si>
+  <si>
+    <t>5.0.2</t>
   </si>
 </sst>
 </file>
@@ -132,12 +165,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -155,11 +188,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -211,19 +239,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -774,21 +802,22 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="12.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="12.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="24.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="15.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="11.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -803,6 +832,49 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Test Suite, Test cases to skip\run
Select Test Suite, Test cases to skip\run
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="7980" activeTab="2"/>
+    <workbookView windowWidth="20370" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>TCID</t>
   </si>
@@ -37,6 +37,15 @@
     <t>Y</t>
   </si>
   <si>
+    <t>RaiseTicketTest</t>
+  </si>
+  <si>
+    <t>Test Cases for Raising the ticket</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>ALPHA_LIST_CAPS</t>
   </si>
   <si>
@@ -59,9 +68,6 @@
   </si>
   <si>
     <t>CCC</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>DDD</t>
@@ -606,13 +612,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="12.1428571428571" style="6" customWidth="1"/>
     <col min="2" max="2" width="43.2857142857143" style="6" customWidth="1"/>
@@ -640,6 +646,17 @@
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -668,23 +685,23 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -692,27 +709,27 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -720,34 +737,34 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -755,27 +772,27 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -783,13 +800,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -802,79 +819,90 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="24.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="11.5714285714286" customWidth="1"/>
+    <col min="7" max="7" width="13.2857142857143" customWidth="1"/>
+    <col min="8" max="8" width="27.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>